<commit_message>
Updated Excel doc and added comment
</commit_message>
<xml_diff>
--- a/data/sum_of_data.xlsx
+++ b/data/sum_of_data.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="18">
   <si>
     <t>Time to load in the TLP</t>
   </si>
@@ -78,6 +78,9 @@
   </si>
   <si>
     <t>Total Time Standard Deviation</t>
+  </si>
+  <si>
+    <t>Edge-based Bundling</t>
   </si>
 </sst>
 </file>
@@ -310,7 +313,7 @@
                   <c:v>None</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Edge</c:v>
+                  <c:v>Edge-based Bundling</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>Pruning</c:v>
@@ -437,7 +440,7 @@
                   <c:v>None</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Edge</c:v>
+                  <c:v>Edge-based Bundling</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>Pruning</c:v>
@@ -564,7 +567,7 @@
                   <c:v>None</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Edge</c:v>
+                  <c:v>Edge-based Bundling</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>Pruning</c:v>
@@ -691,7 +694,7 @@
                   <c:v>None</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Edge</c:v>
+                  <c:v>Edge-based Bundling</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>Pruning</c:v>
@@ -1205,7 +1208,7 @@
                   <c:v>None</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Edge</c:v>
+                  <c:v>Edge-based Bundling</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>Pruning</c:v>
@@ -1332,7 +1335,7 @@
                   <c:v>None</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Edge</c:v>
+                  <c:v>Edge-based Bundling</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>Pruning</c:v>
@@ -1459,7 +1462,7 @@
                   <c:v>None</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Edge</c:v>
+                  <c:v>Edge-based Bundling</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>Pruning</c:v>
@@ -1586,7 +1589,7 @@
                   <c:v>None</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Edge</c:v>
+                  <c:v>Edge-based Bundling</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>Pruning</c:v>
@@ -5338,15 +5341,15 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>609599</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>23282</xdr:colOff>
+      <xdr:row>26</xdr:row>
       <xdr:rowOff>165100</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -5452,16 +5455,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>603250</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>107950</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>165100</xdr:rowOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5757,13 +5760,15 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="29.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="5" width="8.7265625" customWidth="1"/>
+    <col min="2" max="2" width="8.7265625" customWidth="1"/>
+    <col min="3" max="3" width="18.36328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="8.7265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
@@ -5772,7 +5777,7 @@
         <v>10</v>
       </c>
       <c r="C1" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="D1" t="s">
         <v>11</v>
@@ -7606,8 +7611,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>